<commit_message>
updated the SDK interface
git-svn-id: https://svn.cs.biu.ac.il/svn/development/SDK@50 ba1fec17-5bc3-4c1d-a110-6a66ae20c876
</commit_message>
<xml_diff>
--- a/Docs/SDK_interface.xlsx
+++ b/Docs/SDK_interface.xlsx
@@ -13,14 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="SecureRandom" localSheetId="0">Sheet1!$D$10</definedName>
-    <definedName name="Signature" localSheetId="0">Sheet1!$D$63</definedName>
+    <definedName name="Signature" localSheetId="0">Sheet1!$D$122</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="169">
   <si>
     <t>Pseudorandom generator</t>
   </si>
@@ -73,9 +73,6 @@
     <t>getBlockSize()</t>
   </si>
   <si>
-    <t>processBlock(byte[], int, byte[], int)</t>
-  </si>
-  <si>
     <t>reset()</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>returnByte(byte)</t>
   </si>
   <si>
-    <t>processBytes(byte[], int, int, byte[], int)</t>
-  </si>
-  <si>
     <t>Digest</t>
   </si>
   <si>
@@ -319,9 +313,6 @@
     <t>AsymetricEncryption</t>
   </si>
   <si>
-    <t>??? Why use a different interface</t>
-  </si>
-  <si>
     <t>DigitalSignature</t>
   </si>
   <si>
@@ -329,13 +320,241 @@
   </si>
   <si>
     <t>SignatureSpi</t>
+  </si>
+  <si>
+    <t>Performs a final update on the digest using the specified array of bytes, then completes the digest computation.</t>
+  </si>
+  <si>
+    <t>Completes the hash computation by performing final operations such as padding</t>
+  </si>
+  <si>
+    <t> Updates the digest using the specified array of bytes.</t>
+  </si>
+  <si>
+    <t>Updates the digest using the specified array of bytes, starting at the specified offset.</t>
+  </si>
+  <si>
+    <t>Generates a user-specified number of random bytes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reseeds this random object, using the eight bytes contained in the given </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>long seed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Reseeds this random object.</t>
+  </si>
+  <si>
+    <t>Generates a SecureRandom object that implements the specified Pseudo Random Number Generator (PRNG) algorithm.</t>
+  </si>
+  <si>
+    <t>Completes the MAC computation and resets the MAC for further use, maintaining the secret key that the MAC was initialized with.</t>
+  </si>
+  <si>
+    <t>Processes the given byte.</t>
+  </si>
+  <si>
+    <t>Initializes the MAC with the given (secret) key and algorithm parameters.</t>
+  </si>
+  <si>
+    <t>esets the MAC for further use, maintaining the secret key that the MAC was initialized with.</t>
+  </si>
+  <si>
+    <t>Continues a multiple-part encryption or decryption operation (depending on how this cipher was initialized), processing another data part.</t>
+  </si>
+  <si>
+    <t>Encrypts or decrypts data in a single-part operation, or finishes a multiple-part operation.</t>
+  </si>
+  <si>
+    <t>Verifies the passed-in signature.</t>
+  </si>
+  <si>
+    <t>Returns the signature bytes of all the data updated so far.</t>
+  </si>
+  <si>
+    <t>Updates the data to be signed or verified using the specified byte.</t>
+  </si>
+  <si>
+    <t>process a block of bytes from in putting the result into out.</t>
+  </si>
+  <si>
+    <t>processBytes(byte[] in , int, int, byte[] out, int)</t>
+  </si>
+  <si>
+    <t>encrypt/decrypt a single byte returning the result.</t>
+  </si>
+  <si>
+    <t>Initialise the cipher.</t>
+  </si>
+  <si>
+    <t>Initialise the cipher.CipherParameters -  the key and other data required by the cipher</t>
+  </si>
+  <si>
+    <t>Process one block of input from the array in and write it to the out array.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">processBlock(byte[] in, int inOff, byte[] out, int outOff) </t>
+  </si>
+  <si>
+    <t>close the digest, producing the final digest value.</t>
+  </si>
+  <si>
+    <t>update the message digest with a block of bytes.</t>
+  </si>
+  <si>
+    <t>reset the digest back to it's initial state.</t>
+  </si>
+  <si>
+    <t>add a single byte to the mac for processing.</t>
+  </si>
+  <si>
+    <t>Compute the final stage of the MAC writing the output to the out parameter.</t>
+  </si>
+  <si>
+    <t>process the block of len bytes stored in in from offset inOff.</t>
+  </si>
+  <si>
+    <t>returns the largest size an input block can be.</t>
+  </si>
+  <si>
+    <t>return true if the internal state represents the signature described in the passed in array.</t>
+  </si>
+  <si>
+    <t>update the internal digest with the byte array in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update(byte[] in, int off, int len) </t>
+  </si>
+  <si>
+    <t>generate a signature for the message we've been loaded with using the key we were initialised with.</t>
+  </si>
+  <si>
+    <t>SDK Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">encryptBlock(byte[] in, int inOff, byte[] out, int outOff) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">decryptBlock(byte[] in, int inOff, byte[] out, int outOff) </t>
+  </si>
+  <si>
+    <t>return the algorithm name</t>
+  </si>
+  <si>
+    <t>returns the block size</t>
+  </si>
+  <si>
+    <t>encrypts the dara</t>
+  </si>
+  <si>
+    <t>decrypts the dara</t>
+  </si>
+  <si>
+    <t>inits the PRG with relevant parameters</t>
+  </si>
+  <si>
+    <t>streamBytes(byte[] in , int, int, byte[] out, int)</t>
+  </si>
+  <si>
+    <t>XOR a single byte</t>
+  </si>
+  <si>
+    <t>hashDatal()</t>
+  </si>
+  <si>
+    <t>insertMsg(byte[] msg)</t>
+  </si>
+  <si>
+    <t>getHashedMsgSize()</t>
+  </si>
+  <si>
+    <t>the output size</t>
+  </si>
+  <si>
+    <t>insert the message to hash</t>
+  </si>
+  <si>
+    <t>hashDatal(byte[] msg)</t>
+  </si>
+  <si>
+    <t>hash message msg</t>
+  </si>
+  <si>
+    <t>hash the message that was inserted by the call to insertMsg</t>
+  </si>
+  <si>
+    <t>PRNG</t>
+  </si>
+  <si>
+    <t>DLOG</t>
+  </si>
+  <si>
+    <t>Get generator</t>
+  </si>
+  <si>
+    <t>Get random element</t>
+  </si>
+  <si>
+    <t>Add and multiply mod q</t>
+  </si>
+  <si>
+    <t>Compute inverse of a group element</t>
+  </si>
+  <si>
+    <t>Exponentiate</t>
+  </si>
+  <si>
+    <t>Multiple exponentiations with same base</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Multiply group elements</t>
+  </si>
+  <si>
+    <t>grhs computations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilinear operations </t>
+  </si>
+  <si>
+    <t>Taken from the file : primitives_for_implementationV2.2.docx</t>
+  </si>
+  <si>
+    <t>getRandom|(int randomSize)</t>
+  </si>
+  <si>
+    <t>invoke the stream cipher on the incloming bytes (it is not relevant if we encrypt or decrypt - same operation)</t>
+  </si>
+  <si>
+    <t>streamSingleByte(byte)</t>
+  </si>
+  <si>
+    <t>PRP (the same as PRF)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +584,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -413,7 +638,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +669,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,21 +739,23 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -820,20 +1053,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:S112"/>
+  <dimension ref="B2:S171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="40.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.125" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.125" customWidth="1"/>
+    <col min="4" max="4" width="35.75" customWidth="1"/>
+    <col min="5" max="5" width="52.125" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="56.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.25" customWidth="1"/>
     <col min="14" max="14" width="3.375" customWidth="1"/>
     <col min="15" max="18" width="9" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="42" customWidth="1"/>
@@ -848,14 +1081,14 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="19.5" thickTop="1" thickBot="1">
@@ -865,14 +1098,14 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="19.5" thickTop="1" thickBot="1">
@@ -886,10 +1119,10 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="S5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:19" ht="19.5" thickTop="1" thickBot="1">
@@ -899,11 +1132,11 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="S6" t="s">
         <v>5</v>
@@ -918,11 +1151,11 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="19.5" thickTop="1" thickBot="1">
@@ -931,14 +1164,14 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="19.5" thickTop="1" thickBot="1">
@@ -952,7 +1185,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="19.5" thickTop="1" thickBot="1">
@@ -964,7 +1197,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="15" thickTop="1"/>
@@ -975,7 +1208,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="F14" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -990,7 +1223,7 @@
     </row>
     <row r="16" spans="2:19" ht="15">
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="4"/>
@@ -1003,7 +1236,9 @@
       <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" t="s">
+        <v>121</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1021,9 +1256,11 @@
     <row r="19" spans="2:8" ht="15">
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>119</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1031,9 +1268,11 @@
     <row r="20" spans="2:8" ht="15">
       <c r="B20" s="2"/>
       <c r="C20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="4"/>
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
+        <v>117</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1041,7 +1280,7 @@
     <row r="21" spans="2:8" ht="15">
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4"/>
       <c r="F21" s="3"/>
@@ -1071,7 +1310,9 @@
       <c r="C24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" t="s">
+        <v>120</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1099,9 +1340,11 @@
     <row r="27" spans="2:8" ht="15">
       <c r="B27" s="2"/>
       <c r="C27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="4"/>
+        <v>123</v>
+      </c>
+      <c r="D27" t="s">
+        <v>122</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1109,7 +1352,7 @@
     <row r="28" spans="2:8" ht="15">
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" s="4"/>
       <c r="F28" s="3"/>
@@ -1126,7 +1369,7 @@
     </row>
     <row r="30" spans="2:8" ht="15">
       <c r="B30" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="4"/>
@@ -1144,69 +1387,82 @@
       <c r="D31" s="4"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="2:8" ht="15">
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D32" s="4"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H32" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="H32" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="33" spans="2:8" ht="15">
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D33" s="4"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H33" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="H33" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="34" spans="2:8" ht="15">
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>125</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H34" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="H34" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="35" spans="2:8" ht="15">
       <c r="B35" s="2"/>
       <c r="C35" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>124</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H35" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="H35" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="36" spans="2:8" ht="15">
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D36" t="s">
+        <v>126</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H36" s="3"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="37" spans="2:8" ht="15">
       <c r="B37" s="4"/>
@@ -1214,7 +1470,7 @@
       <c r="D37" s="4"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H37" s="3"/>
     </row>
@@ -1224,29 +1480,35 @@
       <c r="D38" s="4"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
+    <row r="39" spans="2:8" ht="15">
+      <c r="B39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="4"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+    <row r="40" spans="2:8" ht="15">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D40" s="4"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="2:8" ht="15">
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="D41" s="4"/>
       <c r="F41" s="2" t="s">
         <v>11</v>
@@ -1255,24 +1517,30 @@
       <c r="H41" s="3"/>
     </row>
     <row r="42" spans="2:8" ht="15">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="D42" s="4"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="2:8" ht="15">
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="D43" s="4"/>
       <c r="F43" s="2"/>
       <c r="G43" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="H43" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="44" spans="2:8" ht="15">
       <c r="B44" s="4"/>
@@ -1280,19 +1548,23 @@
       <c r="D44" s="4"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="2:8" ht="15">
+        <v>39</v>
+      </c>
+      <c r="H44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="15.75">
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H45" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="H45" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="46" spans="2:8" ht="15">
       <c r="B46" s="4"/>
@@ -1300,9 +1572,11 @@
       <c r="D46" s="4"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H46" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="H46" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="4"/>
@@ -1312,532 +1586,984 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="56" spans="2:7" ht="44.25">
-      <c r="B56" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" ht="15" thickBot="1"/>
-    <row r="58" spans="2:7" s="10" customFormat="1" ht="21.75" thickTop="1" thickBot="1">
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
-      <c r="B59" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
-      <c r="B60" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E60" s="1" t="s">
+    <row r="51" spans="2:4" ht="33.75">
+      <c r="B51" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+    </row>
+    <row r="53" spans="2:4" ht="15">
+      <c r="B53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="2:4" ht="15">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
-      <c r="B61" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
-      <c r="B62" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
-      <c r="B63" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" ht="15" thickTop="1"/>
-    <row r="70" spans="2:8" ht="33.75">
-      <c r="B70" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="F70" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-    </row>
-    <row r="71" spans="2:8">
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-    </row>
-    <row r="72" spans="2:8">
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-    </row>
-    <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="15">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" ht="15">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="15">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" ht="15">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+    </row>
+    <row r="61" spans="2:4" ht="15">
+      <c r="B61" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="2:4" ht="15">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="4"/>
-      <c r="F73" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G73" s="2"/>
-      <c r="H73" s="3"/>
-    </row>
-    <row r="74" spans="2:8" ht="15">
+      <c r="D62" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="15">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="15">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="15">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" ht="15">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+    </row>
+    <row r="69" spans="2:4" ht="15">
+      <c r="B69" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="2:4" ht="15">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="2:4" ht="15">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="2:4" ht="15">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" ht="15">
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" ht="15">
       <c r="B74" s="2"/>
-      <c r="C74" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D74" s="4"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H74" s="3"/>
-    </row>
-    <row r="75" spans="2:8" ht="15">
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="2:4" ht="15">
       <c r="B75" s="2"/>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+    </row>
+    <row r="78" spans="2:4" ht="15">
+      <c r="B78" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="2:4" ht="15">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D75" s="4"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H75" s="3"/>
-    </row>
-    <row r="76" spans="2:8" ht="15">
-      <c r="B76" s="2"/>
-      <c r="C76" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D76" s="4"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H76" s="3"/>
-    </row>
-    <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="2"/>
-      <c r="C77" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D77" s="4"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H77" s="3"/>
-    </row>
-    <row r="78" spans="2:8" ht="15">
-      <c r="B78" s="2"/>
-      <c r="C78" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D78" s="4"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H78" s="3"/>
-    </row>
-    <row r="79" spans="2:8" ht="15">
-      <c r="B79" s="2"/>
-      <c r="C79" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D79" s="4"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H79" s="3"/>
-    </row>
-    <row r="80" spans="2:8" ht="15">
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="2:4" ht="15">
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D80" s="4"/>
-      <c r="H80" s="3"/>
-    </row>
-    <row r="81" spans="2:8">
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
-      <c r="H81" s="3"/>
-    </row>
-    <row r="82" spans="2:8" ht="15">
-      <c r="B82" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C82" s="2"/>
-      <c r="D82" s="4"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-    </row>
-    <row r="83" spans="2:8" ht="15">
+        <v>147</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" ht="15">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" ht="15">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" ht="15">
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D83" s="4"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-    </row>
-    <row r="84" spans="2:8" ht="15">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D84" s="4"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
-    </row>
-    <row r="85" spans="2:8" ht="15">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D85" s="4"/>
-      <c r="F85" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G85" s="2"/>
-      <c r="H85" s="3"/>
-    </row>
-    <row r="86" spans="2:8" ht="15">
-      <c r="B86" s="2"/>
-      <c r="C86" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D86" s="4"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H86" s="3"/>
-    </row>
-    <row r="87" spans="2:8" ht="15">
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H87" s="3"/>
-    </row>
-    <row r="88" spans="2:8" ht="15">
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H88" s="3"/>
-    </row>
-    <row r="89" spans="2:8" ht="15">
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H89" s="3"/>
-    </row>
-    <row r="90" spans="2:8" ht="15">
-      <c r="B90" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C90" s="2"/>
-      <c r="D90" s="4"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H90" s="3"/>
-    </row>
-    <row r="91" spans="2:8" ht="15">
+        <v>145</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+    </row>
+    <row r="86" spans="2:4" ht="15">
+      <c r="B86" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="2:4" ht="15">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="2:4" ht="15">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="2:4" ht="15">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="2:4" ht="15">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="2:4" ht="15">
       <c r="B91" s="2"/>
       <c r="C91" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+    </row>
+    <row r="94" spans="2:4" ht="15">
+      <c r="B94" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="2:4" ht="15">
+      <c r="B95" s="2"/>
+      <c r="C95" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+    </row>
+    <row r="98" spans="2:4" ht="15">
+      <c r="B98" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="2:4" ht="15">
+      <c r="B99" s="2"/>
+      <c r="C99" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" ht="15">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="2:4" ht="15">
+      <c r="B101" s="2"/>
+      <c r="C101" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="2:4" ht="15">
+      <c r="B102" s="2"/>
+      <c r="C102" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="2:4" ht="15">
+      <c r="B103" s="2"/>
+      <c r="C103" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="2:4" ht="15">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="2:4" ht="15">
+      <c r="B105" s="2"/>
+      <c r="C105" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="2:4" ht="15">
+      <c r="B106" s="2"/>
+      <c r="C106" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="2:4" ht="15">
+      <c r="B107" s="2"/>
+      <c r="C107" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="2:4">
+      <c r="B108" s="14"/>
+      <c r="C108" s="14"/>
+      <c r="D108" s="14"/>
+    </row>
+    <row r="109" spans="2:4">
+      <c r="B109" s="14"/>
+      <c r="C109" s="14"/>
+      <c r="D109" s="14"/>
+    </row>
+    <row r="110" spans="2:4">
+      <c r="B110" s="14"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="14"/>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="14"/>
+    </row>
+    <row r="115" spans="2:7" ht="44.25">
+      <c r="B115" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" ht="15" thickBot="1"/>
+    <row r="117" spans="2:7" s="10" customFormat="1" ht="21.75" thickTop="1" thickBot="1">
+      <c r="B117" s="9"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F117" s="9"/>
+      <c r="G117" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
+      <c r="B118" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
+      <c r="B119" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
+      <c r="B120" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
+      <c r="B121" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+    </row>
+    <row r="122" spans="2:7" ht="21.75" thickTop="1" thickBot="1">
+      <c r="B122" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" ht="15" thickTop="1"/>
+    <row r="129" spans="2:8" ht="33.75">
+      <c r="B129" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="F129" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
+    </row>
+    <row r="130" spans="2:8">
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
+      <c r="H130" s="3"/>
+    </row>
+    <row r="131" spans="2:8">
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
+      <c r="H131" s="3"/>
+    </row>
+    <row r="132" spans="2:8" ht="15">
+      <c r="B132" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C132" s="2"/>
+      <c r="D132" s="4"/>
+      <c r="F132" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G132" s="2"/>
+      <c r="H132" s="3"/>
+    </row>
+    <row r="133" spans="2:8" ht="15">
+      <c r="B133" s="2"/>
+      <c r="C133" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D133" s="4"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H133" s="3"/>
+    </row>
+    <row r="134" spans="2:8" ht="15">
+      <c r="B134" s="2"/>
+      <c r="C134" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="4"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H134" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" ht="15">
+      <c r="B135" s="2"/>
+      <c r="C135" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D135" s="4"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H135" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" ht="15">
+      <c r="B136" s="2"/>
+      <c r="C136" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D136" t="s">
+        <v>127</v>
+      </c>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H136" s="3"/>
+    </row>
+    <row r="137" spans="2:8" ht="15">
+      <c r="B137" s="2"/>
+      <c r="C137" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D137" s="4"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H137" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" ht="15">
+      <c r="B138" s="2"/>
+      <c r="C138" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D138" t="s">
+        <v>128</v>
+      </c>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H138" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="139" spans="2:8" ht="15">
+      <c r="B139" s="2"/>
+      <c r="C139" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H139" s="3"/>
+    </row>
+    <row r="140" spans="2:8">
+      <c r="B140" s="4"/>
+      <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
+      <c r="H140" s="3"/>
+    </row>
+    <row r="141" spans="2:8" ht="15">
+      <c r="B141" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C141" s="2"/>
+      <c r="D141" s="4"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="3"/>
+    </row>
+    <row r="142" spans="2:8" ht="15">
+      <c r="B142" s="2"/>
+      <c r="C142" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D91" s="4"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2" t="s">
+      <c r="D142" s="4"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="3"/>
+      <c r="H142" s="3"/>
+    </row>
+    <row r="143" spans="2:8" ht="15">
+      <c r="B143" s="2"/>
+      <c r="C143" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D143" t="s">
+        <v>130</v>
+      </c>
+      <c r="F143" s="3"/>
+      <c r="G143" s="3"/>
+      <c r="H143" s="3"/>
+    </row>
+    <row r="144" spans="2:8" ht="15">
+      <c r="B144" s="2"/>
+      <c r="C144" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D144" s="4"/>
+      <c r="F144" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G144" s="2"/>
+      <c r="H144" s="3"/>
+    </row>
+    <row r="145" spans="2:8" ht="15">
+      <c r="B145" s="2"/>
+      <c r="C145" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D145" t="s">
+        <v>129</v>
+      </c>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H145" s="3"/>
+    </row>
+    <row r="146" spans="2:8" ht="15">
+      <c r="B146" s="4"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H146" s="3"/>
+    </row>
+    <row r="147" spans="2:8" ht="15">
+      <c r="B147" s="4"/>
+      <c r="C147" s="4"/>
+      <c r="D147" s="4"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H147" s="3"/>
+    </row>
+    <row r="148" spans="2:8" ht="15">
+      <c r="B148" s="4"/>
+      <c r="C148" s="4"/>
+      <c r="D148" s="4"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H148" s="3"/>
+    </row>
+    <row r="149" spans="2:8" ht="15">
+      <c r="B149" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C149" s="2"/>
+      <c r="D149" s="4"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H149" s="3"/>
+    </row>
+    <row r="150" spans="2:8" ht="15">
+      <c r="B150" s="2"/>
+      <c r="C150" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D150" s="4"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H150" s="3"/>
+    </row>
+    <row r="151" spans="2:8" ht="15">
+      <c r="B151" s="2"/>
+      <c r="C151" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D151" s="4"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H151" s="3"/>
+    </row>
+    <row r="152" spans="2:8" ht="15">
+      <c r="B152" s="2"/>
+      <c r="C152" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D152" t="s">
+        <v>132</v>
+      </c>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H91" s="3"/>
-    </row>
-    <row r="92" spans="2:8" ht="15">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D92" s="4"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2" t="s">
+      <c r="H152" s="3"/>
+    </row>
+    <row r="153" spans="2:8" ht="15">
+      <c r="B153" s="2"/>
+      <c r="C153" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D153" t="s">
+        <v>134</v>
+      </c>
+      <c r="F153" s="2"/>
+      <c r="G153" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H92" s="3"/>
-    </row>
-    <row r="93" spans="2:8" ht="15">
-      <c r="B93" s="2"/>
-      <c r="C93" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D93" s="4"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2" t="s">
+      <c r="H153" s="3"/>
+    </row>
+    <row r="154" spans="2:8" ht="15">
+      <c r="B154" s="2"/>
+      <c r="C154" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D154" t="s">
+        <v>131</v>
+      </c>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H154" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="155" spans="2:8" ht="15">
+      <c r="B155" s="2"/>
+      <c r="C155" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D155" s="4"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H93" s="3"/>
-    </row>
-    <row r="94" spans="2:8" ht="15">
-      <c r="B94" s="2"/>
-      <c r="C94" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D94" s="4"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2" t="s">
+      <c r="H155" s="3"/>
+    </row>
+    <row r="156" spans="2:8" ht="15">
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="4"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="H94" s="3"/>
-    </row>
-    <row r="95" spans="2:8" ht="15">
-      <c r="B95" s="2"/>
-      <c r="C95" s="12" t="s">
+      <c r="H156" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8" ht="15">
+      <c r="B157" s="4"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="4"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H157" s="3"/>
+    </row>
+    <row r="158" spans="2:8" ht="15">
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="4"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H158" s="3"/>
+    </row>
+    <row r="159" spans="2:8" ht="15">
+      <c r="B159" s="4"/>
+      <c r="C159" s="4"/>
+      <c r="D159" s="4"/>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H159" s="3"/>
+    </row>
+    <row r="160" spans="2:8" ht="15">
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="4"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H160" s="3"/>
+    </row>
+    <row r="161" spans="2:8" ht="15">
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="4"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+      <c r="H161" s="3"/>
+    </row>
+    <row r="162" spans="2:8">
+      <c r="B162" s="4"/>
+      <c r="C162" s="4"/>
+      <c r="D162" s="4"/>
+      <c r="F162" s="3"/>
+      <c r="G162" s="3"/>
+      <c r="H162" s="3"/>
+    </row>
+    <row r="163" spans="2:8">
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="4"/>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3"/>
+      <c r="H163" s="3"/>
+    </row>
+    <row r="164" spans="2:8" ht="15">
+      <c r="B164" s="4"/>
+      <c r="C164" s="4"/>
+      <c r="D164" s="4"/>
+      <c r="F164" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G164" s="2"/>
+      <c r="H164" s="3"/>
+    </row>
+    <row r="165" spans="2:8" ht="15">
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="4"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D95" s="4"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="2" t="s">
+      <c r="H165" s="3"/>
+    </row>
+    <row r="166" spans="2:8" ht="15">
+      <c r="F166" s="2"/>
+      <c r="G166" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H166" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="167" spans="2:8" ht="15">
+      <c r="F167" s="2"/>
+      <c r="G167" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H167" s="3"/>
+    </row>
+    <row r="168" spans="2:8" ht="15">
+      <c r="F168" s="2"/>
+      <c r="G168" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H168" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="169" spans="2:8" ht="15">
+      <c r="F169" s="2"/>
+      <c r="G169" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H95" s="3"/>
-    </row>
-    <row r="96" spans="2:8" ht="15">
-      <c r="B96" s="2"/>
-      <c r="C96" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D96" s="4"/>
-      <c r="F96" s="2"/>
-      <c r="G96" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H96" s="3"/>
-    </row>
-    <row r="97" spans="2:8" ht="15">
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="H97" s="3"/>
-    </row>
-    <row r="98" spans="2:8" ht="15">
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H98" s="3"/>
-    </row>
-    <row r="99" spans="2:8" ht="15">
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H99" s="3"/>
-    </row>
-    <row r="100" spans="2:8" ht="15">
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H100" s="3"/>
-    </row>
-    <row r="101" spans="2:8" ht="15">
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H101" s="3"/>
-    </row>
-    <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="3"/>
-    </row>
-    <row r="103" spans="2:8">
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="3"/>
-      <c r="H103" s="3"/>
-    </row>
-    <row r="104" spans="2:8">
-      <c r="B104" s="4"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="3"/>
-    </row>
-    <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
-      <c r="F105" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G105" s="2"/>
-      <c r="H105" s="3"/>
-    </row>
-    <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H106" s="3"/>
-    </row>
-    <row r="107" spans="2:8" ht="15">
-      <c r="F107" s="2"/>
-      <c r="G107" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H107" s="3"/>
-    </row>
-    <row r="108" spans="2:8" ht="15">
-      <c r="F108" s="2"/>
-      <c r="G108" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H108" s="3"/>
-    </row>
-    <row r="109" spans="2:8" ht="15">
-      <c r="F109" s="2"/>
-      <c r="G109" s="13" t="s">
+      <c r="H169" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="170" spans="2:8" ht="15">
+      <c r="F170" s="2"/>
+      <c r="G170" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H109" s="3"/>
-    </row>
-    <row r="110" spans="2:8" ht="15">
-      <c r="F110" s="2"/>
-      <c r="G110" s="12" t="s">
+      <c r="H170" s="3"/>
+    </row>
+    <row r="171" spans="2:8" ht="15">
+      <c r="F171" s="2"/>
+      <c r="G171" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H110" s="3"/>
-    </row>
-    <row r="111" spans="2:8" ht="15">
-      <c r="F111" s="2"/>
-      <c r="G111" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H111" s="3"/>
-    </row>
-    <row r="112" spans="2:8" ht="15">
-      <c r="F112" s="2"/>
-      <c r="G112" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H112" s="3"/>
+      <c r="H171" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>